<commit_message>
update threshold for PanoramiR
</commit_message>
<xml_diff>
--- a/resources/miRThreshold.xlsx
+++ b/resources/miRThreshold.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIRNB1903\Desktop\PanoramiR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plateau/Documents/GitHub/PanoramiR/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B769220C-9115-49F2-9F25-A7AA3420CF11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49ECB92B-ACC4-3746-BEEA-8F7CD96259E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2CC14BC5-EBA4-42DD-B94E-4879B9B90E01}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12580" xr2:uid="{2CC14BC5-EBA4-42DD-B94E-4879B9B90E01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1198,7 +1198,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1206,13 +1206,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFACA47"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1227,8 +1241,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1546,12 +1563,12 @@
   <dimension ref="A1:B385"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A385"/>
+      <selection activeCell="B2" sqref="B2:B385"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>385</v>
       </c>
@@ -1559,3076 +1576,3076 @@
         <v>384</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B22">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B23">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B24">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="B27">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="B28">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="B29">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
-      <c r="B30">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
-      <c r="B31">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B31" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
-      <c r="B32">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B32" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
-      <c r="B33">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
-      <c r="B34">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
-      <c r="B35">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
-      <c r="B37">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
-      <c r="B38">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
-      <c r="B39">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
-      <c r="B40">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="B41">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>40</v>
       </c>
-      <c r="B42">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B42" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
-      <c r="B43">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B43" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>42</v>
       </c>
-      <c r="B44">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B44" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
-      <c r="B45">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B45" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>44</v>
       </c>
-      <c r="B46">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B46" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>45</v>
       </c>
-      <c r="B47">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
-      <c r="B48">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B48" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>47</v>
       </c>
-      <c r="B49">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>48</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
-      <c r="B51">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>50</v>
       </c>
-      <c r="B52">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>51</v>
       </c>
-      <c r="B53">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B53" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
-      <c r="B54">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B54" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
-      <c r="B55">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B55" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>54</v>
       </c>
-      <c r="B56">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B56" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>55</v>
       </c>
-      <c r="B57">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>56</v>
       </c>
-      <c r="B58">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B58" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>57</v>
       </c>
-      <c r="B59">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B59" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
-      <c r="B60">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B60" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>59</v>
       </c>
-      <c r="B61">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B61" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>60</v>
       </c>
-      <c r="B62">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B62" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>61</v>
       </c>
-      <c r="B63">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B63" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>62</v>
       </c>
-      <c r="B64">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B64" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>63</v>
       </c>
-      <c r="B65">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B65" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
       </c>
-      <c r="B66">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B66" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
-      <c r="B67">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B67" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>66</v>
       </c>
-      <c r="B68">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B68" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>67</v>
       </c>
-      <c r="B69">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>68</v>
       </c>
-      <c r="B70">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B70" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>69</v>
       </c>
-      <c r="B71">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B71" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>70</v>
       </c>
-      <c r="B72">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B72" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>71</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>72</v>
       </c>
-      <c r="B74">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B74" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>73</v>
       </c>
-      <c r="B75">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B75" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>74</v>
       </c>
-      <c r="B76">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B76" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>75</v>
       </c>
-      <c r="B77">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B77" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>76</v>
       </c>
-      <c r="B78">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B78" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>77</v>
       </c>
-      <c r="B79">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B79" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>78</v>
       </c>
-      <c r="B80">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B80" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>79</v>
       </c>
-      <c r="B81">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B81" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>80</v>
       </c>
-      <c r="B82">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B82" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>81</v>
       </c>
-      <c r="B83">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B83" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>82</v>
       </c>
-      <c r="B84">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>83</v>
       </c>
-      <c r="B85">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B85" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>84</v>
       </c>
-      <c r="B86">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B86" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>85</v>
       </c>
-      <c r="B87">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B87" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>86</v>
       </c>
-      <c r="B88">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B88" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>87</v>
       </c>
-      <c r="B89">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B89" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>88</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>89</v>
       </c>
-      <c r="B91">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B91" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>90</v>
       </c>
-      <c r="B92">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B92" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>91</v>
       </c>
-      <c r="B93">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B93" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>92</v>
       </c>
-      <c r="B94">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B94" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>93</v>
       </c>
-      <c r="B95">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B95" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>94</v>
       </c>
-      <c r="B96">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B96" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>95</v>
       </c>
-      <c r="B97">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B97" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>96</v>
       </c>
-      <c r="B98">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B98" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>97</v>
       </c>
-      <c r="B99">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B99" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>98</v>
       </c>
-      <c r="B100">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B100" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>99</v>
       </c>
-      <c r="B101">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B101" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>100</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>101</v>
       </c>
-      <c r="B103">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B103" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>102</v>
       </c>
-      <c r="B104">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B104" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>103</v>
       </c>
-      <c r="B105">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B105" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>104</v>
       </c>
-      <c r="B106">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B106" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>105</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>106</v>
       </c>
-      <c r="B108">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B108" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>107</v>
       </c>
-      <c r="B109">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B109" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>108</v>
       </c>
-      <c r="B110">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B110" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>109</v>
       </c>
-      <c r="B111">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B111" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>110</v>
       </c>
-      <c r="B112">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B112" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>111</v>
       </c>
-      <c r="B113">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B113" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>112</v>
       </c>
-      <c r="B114">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B114" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>113</v>
       </c>
-      <c r="B115">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B115" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>114</v>
       </c>
-      <c r="B116">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B116" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>115</v>
       </c>
-      <c r="B117">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B117" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>116</v>
       </c>
-      <c r="B118">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B118" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>117</v>
       </c>
-      <c r="B119">
+      <c r="B119" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>118</v>
       </c>
-      <c r="B120">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B120" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>119</v>
       </c>
-      <c r="B121">
+      <c r="B121" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>120</v>
       </c>
-      <c r="B122">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B122" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>121</v>
       </c>
-      <c r="B123">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B123" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>122</v>
       </c>
-      <c r="B124">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B124" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>123</v>
       </c>
-      <c r="B125">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B125" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>124</v>
       </c>
-      <c r="B126">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B126" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>125</v>
       </c>
-      <c r="B127">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B127" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>126</v>
       </c>
-      <c r="B128">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B128" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>127</v>
       </c>
-      <c r="B129">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B129" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>128</v>
       </c>
-      <c r="B130">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B130" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>129</v>
       </c>
-      <c r="B131">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B131" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>130</v>
       </c>
-      <c r="B132">
+      <c r="B132" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>131</v>
       </c>
-      <c r="B133">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B133" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>132</v>
       </c>
-      <c r="B134">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B134" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>133</v>
       </c>
-      <c r="B135">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B135" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>134</v>
       </c>
-      <c r="B136">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B136" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>135</v>
       </c>
-      <c r="B137">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B137" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>136</v>
       </c>
-      <c r="B138">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B138" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>137</v>
       </c>
-      <c r="B139">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B139" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>138</v>
       </c>
-      <c r="B140">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B140" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>139</v>
       </c>
-      <c r="B141">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B141" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>140</v>
       </c>
-      <c r="B142">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B142" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>141</v>
       </c>
-      <c r="B143">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B143" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>142</v>
       </c>
-      <c r="B144">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B144" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>143</v>
       </c>
-      <c r="B145">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B145" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>144</v>
       </c>
-      <c r="B146">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B146" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>145</v>
       </c>
-      <c r="B147">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B147" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>146</v>
       </c>
-      <c r="B148">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B148" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>147</v>
       </c>
-      <c r="B149">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B149" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>148</v>
       </c>
-      <c r="B150">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B150" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>149</v>
       </c>
-      <c r="B151">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B151" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>150</v>
       </c>
-      <c r="B152">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B152" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>151</v>
       </c>
-      <c r="B153">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B153" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>152</v>
       </c>
-      <c r="B154">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B154" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>153</v>
       </c>
-      <c r="B155">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B155" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>154</v>
       </c>
-      <c r="B156">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B156" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>155</v>
       </c>
-      <c r="B157">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B157" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>156</v>
       </c>
-      <c r="B158">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B158" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>157</v>
       </c>
-      <c r="B159">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B159" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>158</v>
       </c>
-      <c r="B160">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B160" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>159</v>
       </c>
-      <c r="B161">
+      <c r="B161" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>160</v>
       </c>
-      <c r="B162">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B162" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>161</v>
       </c>
-      <c r="B163">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B163" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>162</v>
       </c>
-      <c r="B164">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B164" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>163</v>
       </c>
-      <c r="B165">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B165" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>164</v>
       </c>
-      <c r="B166">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B166" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>165</v>
       </c>
-      <c r="B167">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B167" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>166</v>
       </c>
-      <c r="B168">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B168" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>167</v>
       </c>
-      <c r="B169">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B169" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>168</v>
       </c>
-      <c r="B170">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B170" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>169</v>
       </c>
-      <c r="B171">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B171" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>170</v>
       </c>
-      <c r="B172">
+      <c r="B172" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>171</v>
       </c>
-      <c r="B173">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B173" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>172</v>
       </c>
-      <c r="B174">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B174" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>173</v>
       </c>
-      <c r="B175">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B175" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>174</v>
       </c>
-      <c r="B176">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B176" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>175</v>
       </c>
-      <c r="B177">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B177" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>176</v>
       </c>
-      <c r="B178">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B178" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>177</v>
       </c>
-      <c r="B179">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B179" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>178</v>
       </c>
-      <c r="B180">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B180" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>179</v>
       </c>
-      <c r="B181">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B181" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>180</v>
       </c>
-      <c r="B182">
+      <c r="B182" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>181</v>
       </c>
-      <c r="B183">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B183" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>182</v>
       </c>
-      <c r="B184">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B184" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>183</v>
       </c>
-      <c r="B185">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B185" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>184</v>
       </c>
-      <c r="B186">
+      <c r="B186" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>185</v>
       </c>
-      <c r="B187">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B187" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>186</v>
       </c>
-      <c r="B188">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B188" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>187</v>
       </c>
-      <c r="B189">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B189" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>188</v>
       </c>
-      <c r="B190">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B190" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>189</v>
       </c>
-      <c r="B191">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B191" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>190</v>
       </c>
-      <c r="B192">
+      <c r="B192" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>191</v>
       </c>
-      <c r="B193">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B193" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>192</v>
       </c>
-      <c r="B194">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B194" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>193</v>
       </c>
-      <c r="B195">
+      <c r="B195" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>194</v>
       </c>
-      <c r="B196">
+      <c r="B196" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>195</v>
       </c>
-      <c r="B197">
+      <c r="B197" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>196</v>
       </c>
-      <c r="B198">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B198" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>197</v>
       </c>
-      <c r="B199">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B199" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>198</v>
       </c>
-      <c r="B200">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B200" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>199</v>
       </c>
-      <c r="B201">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B201" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>200</v>
       </c>
-      <c r="B202">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B202" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>201</v>
       </c>
-      <c r="B203">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B203" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>202</v>
       </c>
-      <c r="B204">
+      <c r="B204" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>203</v>
       </c>
-      <c r="B205">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B205" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>204</v>
       </c>
-      <c r="B206">
+      <c r="B206" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>205</v>
       </c>
-      <c r="B207">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B207" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>206</v>
       </c>
-      <c r="B208">
+      <c r="B208" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>207</v>
       </c>
-      <c r="B209">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B209" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>208</v>
       </c>
-      <c r="B210">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B210" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>209</v>
       </c>
-      <c r="B211">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B211" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>210</v>
       </c>
-      <c r="B212">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B212" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>211</v>
       </c>
-      <c r="B213">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B213" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>212</v>
       </c>
-      <c r="B214">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B214" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>213</v>
       </c>
-      <c r="B215">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B215" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>214</v>
       </c>
-      <c r="B216">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B216" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>215</v>
       </c>
-      <c r="B217">
+      <c r="B217" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>216</v>
       </c>
-      <c r="B218">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B218" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>217</v>
       </c>
-      <c r="B219">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B219" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>218</v>
       </c>
-      <c r="B220">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B220" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>219</v>
       </c>
-      <c r="B221">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B221" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>220</v>
       </c>
-      <c r="B222">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B222" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>221</v>
       </c>
-      <c r="B223">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B223" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>222</v>
       </c>
-      <c r="B224">
+      <c r="B224" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>223</v>
       </c>
-      <c r="B225">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B225" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>224</v>
       </c>
-      <c r="B226">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B226" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>225</v>
       </c>
-      <c r="B227">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B227" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>226</v>
       </c>
-      <c r="B228">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B228" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>227</v>
       </c>
-      <c r="B229">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B229" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>228</v>
       </c>
-      <c r="B230">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B230" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>229</v>
       </c>
-      <c r="B231">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B231" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>230</v>
       </c>
-      <c r="B232">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B232" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>231</v>
       </c>
-      <c r="B233">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B233" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>232</v>
       </c>
-      <c r="B234">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B234" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>233</v>
       </c>
-      <c r="B235">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B235" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>234</v>
       </c>
-      <c r="B236">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B236" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>235</v>
       </c>
-      <c r="B237">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B237" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>236</v>
       </c>
-      <c r="B238">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B238" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>237</v>
       </c>
-      <c r="B239">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B239" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>238</v>
       </c>
-      <c r="B240">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B240" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>239</v>
       </c>
-      <c r="B241">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B241" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>240</v>
       </c>
-      <c r="B242">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B242" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>241</v>
       </c>
-      <c r="B243">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B243" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>242</v>
       </c>
-      <c r="B244">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B244" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>243</v>
       </c>
-      <c r="B245">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B245" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>244</v>
       </c>
-      <c r="B246">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B246" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>245</v>
       </c>
-      <c r="B247">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B247" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>246</v>
       </c>
-      <c r="B248">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B248" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>247</v>
       </c>
-      <c r="B249">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B249" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>248</v>
       </c>
-      <c r="B250">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B250" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>249</v>
       </c>
-      <c r="B251">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B251" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>250</v>
       </c>
-      <c r="B252">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B252" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>251</v>
       </c>
-      <c r="B253">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B253" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>252</v>
       </c>
-      <c r="B254">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B254" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>253</v>
       </c>
-      <c r="B255">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B255" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>254</v>
       </c>
-      <c r="B256">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B256" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>255</v>
       </c>
-      <c r="B257">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B257" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>256</v>
       </c>
-      <c r="B258">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B258" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>257</v>
       </c>
-      <c r="B259">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B259" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>258</v>
       </c>
-      <c r="B260">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B260" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>259</v>
       </c>
-      <c r="B261">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B261" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>260</v>
       </c>
-      <c r="B262">
+      <c r="B262" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>261</v>
       </c>
-      <c r="B263">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B263" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>262</v>
       </c>
-      <c r="B264">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B264" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>263</v>
       </c>
-      <c r="B265">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B265" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>264</v>
       </c>
-      <c r="B266">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B266" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>265</v>
       </c>
-      <c r="B267">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B267" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>266</v>
       </c>
-      <c r="B268">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B268" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>267</v>
       </c>
-      <c r="B269">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B269" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>268</v>
       </c>
-      <c r="B270">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B270" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>269</v>
       </c>
-      <c r="B271">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B271" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>270</v>
       </c>
-      <c r="B272">
+      <c r="B272" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>271</v>
       </c>
-      <c r="B273">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B273" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>272</v>
       </c>
-      <c r="B274">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B274" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>273</v>
       </c>
-      <c r="B275">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B275" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>274</v>
       </c>
-      <c r="B276">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B276" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>275</v>
       </c>
-      <c r="B277">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B277" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>276</v>
       </c>
-      <c r="B278">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B278" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>277</v>
       </c>
-      <c r="B279">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B279" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>278</v>
       </c>
-      <c r="B280">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B280" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>279</v>
       </c>
-      <c r="B281">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B281" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>280</v>
       </c>
-      <c r="B282">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B282" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>281</v>
       </c>
-      <c r="B283">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B283" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>282</v>
       </c>
-      <c r="B284">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B284" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>283</v>
       </c>
-      <c r="B285">
+      <c r="B285" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>284</v>
       </c>
-      <c r="B286">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B286" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>285</v>
       </c>
-      <c r="B287">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B287" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>286</v>
       </c>
-      <c r="B288">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B288" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>287</v>
       </c>
-      <c r="B289">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B289" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>288</v>
       </c>
-      <c r="B290">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B290" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>289</v>
       </c>
-      <c r="B291">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B291" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>290</v>
       </c>
-      <c r="B292">
+      <c r="B292" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>291</v>
       </c>
-      <c r="B293">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B293" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>292</v>
       </c>
-      <c r="B294">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B294" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>293</v>
       </c>
-      <c r="B295">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B295" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>294</v>
       </c>
-      <c r="B296">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B296" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>295</v>
       </c>
-      <c r="B297">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B297" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>296</v>
       </c>
-      <c r="B298">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B298" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>297</v>
       </c>
-      <c r="B299">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B299" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>298</v>
       </c>
-      <c r="B300">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B300" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>299</v>
       </c>
-      <c r="B301">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B301" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>300</v>
       </c>
-      <c r="B302">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B302" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>301</v>
       </c>
-      <c r="B303">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B303" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>302</v>
       </c>
-      <c r="B304">
+      <c r="B304" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>303</v>
       </c>
-      <c r="B305">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B305" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>304</v>
       </c>
-      <c r="B306">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B306" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>305</v>
       </c>
-      <c r="B307">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B307" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>306</v>
       </c>
-      <c r="B308">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B308" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>307</v>
       </c>
-      <c r="B309">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B309" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>308</v>
       </c>
-      <c r="B310">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B310" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>309</v>
       </c>
-      <c r="B311">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B311" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>310</v>
       </c>
-      <c r="B312">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B312" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>311</v>
       </c>
-      <c r="B313">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B313" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>312</v>
       </c>
-      <c r="B314">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B314" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>313</v>
       </c>
-      <c r="B315">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B315" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>314</v>
       </c>
-      <c r="B316">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B316" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>315</v>
       </c>
-      <c r="B317">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B317" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>316</v>
       </c>
-      <c r="B318">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B318" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>317</v>
       </c>
-      <c r="B319">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B319" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>318</v>
       </c>
-      <c r="B320">
+      <c r="B320" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>319</v>
       </c>
-      <c r="B321">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B321" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>320</v>
       </c>
-      <c r="B322">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B322" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>321</v>
       </c>
-      <c r="B323">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B323" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>322</v>
       </c>
-      <c r="B324">
+      <c r="B324" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>323</v>
       </c>
-      <c r="B325">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B325" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>324</v>
       </c>
-      <c r="B326">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B326" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>325</v>
       </c>
-      <c r="B327">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B327" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>326</v>
       </c>
-      <c r="B328">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B328" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>327</v>
       </c>
-      <c r="B329">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B329" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>328</v>
       </c>
-      <c r="B330">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B330" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>329</v>
       </c>
-      <c r="B331">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B331" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>330</v>
       </c>
-      <c r="B332">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B332" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>331</v>
       </c>
-      <c r="B333">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B333" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>332</v>
       </c>
-      <c r="B334">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B334" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>333</v>
       </c>
-      <c r="B335">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B335" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>334</v>
       </c>
-      <c r="B336">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B336" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>335</v>
       </c>
-      <c r="B337">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B337" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>336</v>
       </c>
-      <c r="B338">
+      <c r="B338" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>337</v>
       </c>
-      <c r="B339">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B339" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>338</v>
       </c>
-      <c r="B340">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B340" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>339</v>
       </c>
-      <c r="B341">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B341" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>340</v>
       </c>
-      <c r="B342">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B342" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>341</v>
       </c>
-      <c r="B343">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B343" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>342</v>
       </c>
-      <c r="B344">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B344" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>343</v>
       </c>
-      <c r="B345">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B345" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>344</v>
       </c>
-      <c r="B346">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B346" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>345</v>
       </c>
-      <c r="B347">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B347" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>346</v>
       </c>
-      <c r="B348">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B348" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>347</v>
       </c>
-      <c r="B349">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B349" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>348</v>
       </c>
-      <c r="B350">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B350" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>349</v>
       </c>
-      <c r="B351">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B351" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>350</v>
       </c>
-      <c r="B352">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B352" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>351</v>
       </c>
-      <c r="B353">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B353" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>352</v>
       </c>
-      <c r="B354">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B354" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>353</v>
       </c>
-      <c r="B355">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B355" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>354</v>
       </c>
-      <c r="B356">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B356" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>355</v>
       </c>
-      <c r="B357">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B357" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>356</v>
       </c>
-      <c r="B358">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B358" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>357</v>
       </c>
-      <c r="B359">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B359" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>358</v>
       </c>
-      <c r="B360">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B360" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>359</v>
       </c>
-      <c r="B361">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B361" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>360</v>
       </c>
-      <c r="B362">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B362" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>361</v>
       </c>
-      <c r="B363">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B363" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>362</v>
       </c>
-      <c r="B364">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B364" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>363</v>
       </c>
-      <c r="B365">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B365" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>364</v>
       </c>
-      <c r="B366">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B366" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>365</v>
       </c>
-      <c r="B367">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B367" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>366</v>
       </c>
-      <c r="B368">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B368" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>367</v>
       </c>
-      <c r="B369">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B369" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>368</v>
       </c>
-      <c r="B370">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B370" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>369</v>
       </c>
-      <c r="B371">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B371" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>370</v>
       </c>
-      <c r="B372">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B372" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>371</v>
       </c>
-      <c r="B373">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B373" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>372</v>
       </c>
-      <c r="B374">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B374" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>373</v>
       </c>
-      <c r="B375">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B375" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>374</v>
       </c>
-      <c r="B376">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B376" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>375</v>
       </c>
-      <c r="B377">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B377" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>376</v>
       </c>
-      <c r="B378">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B378" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>377</v>
       </c>
-      <c r="B379">
+      <c r="B379" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>378</v>
       </c>
-      <c r="B380">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B380" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>379</v>
       </c>
-      <c r="B381">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B381" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>380</v>
       </c>
-      <c r="B382">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B382" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>381</v>
       </c>
-      <c r="B383">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B383" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>382</v>
       </c>
-      <c r="B384">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B384" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>383</v>
       </c>
-      <c r="B385">
-        <v>29</v>
+      <c r="B385" s="1">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>